<commit_message>
add dist as backup
</commit_message>
<xml_diff>
--- a/pollsdata/A/A-abdzadeh.xlsx
+++ b/pollsdata/A/A-abdzadeh.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Sepah\wall_recommender\pollsdata\A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AF3189-26DB-44EA-8193-1966C2C3D1E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448D10C8-C3EF-476B-817B-01B424553581}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16200" yWindow="2070" windowWidth="16200" windowHeight="9810" xr2:uid="{0D50DD6A-70CC-4B93-B041-37A9024A9212}"/>
+    <workbookView xWindow="-16320" yWindow="2730" windowWidth="16200" windowHeight="9810" xr2:uid="{0D50DD6A-70CC-4B93-B041-37A9024A9212}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="29">
   <si>
     <t>نوع دیوار</t>
   </si>
@@ -81,9 +81,6 @@
     <t>بالا</t>
   </si>
   <si>
-    <t>قوی</t>
-  </si>
-  <si>
     <t>دشت</t>
   </si>
   <si>
@@ -96,21 +93,12 @@
     <t>آسان</t>
   </si>
   <si>
-    <t>متوسط</t>
-  </si>
-  <si>
-    <t>ضعیف</t>
-  </si>
-  <si>
     <t>تپه ماهور</t>
   </si>
   <si>
     <t>بله</t>
   </si>
   <si>
-    <t>کوهستان</t>
-  </si>
-  <si>
     <t>بدون محافظ</t>
   </si>
   <si>
@@ -121,6 +109,15 @@
   </si>
   <si>
     <t>درجاریز</t>
+  </si>
+  <si>
+    <t>متراکم</t>
+  </si>
+  <si>
+    <t>سست</t>
+  </si>
+  <si>
+    <t>کوهستانی</t>
   </si>
 </sst>
 </file>
@@ -482,7 +479,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -538,13 +535,13 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -556,16 +553,16 @@
         <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="K2" s="1">
         <v>28</v>
@@ -573,10 +570,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>21</v>
@@ -591,16 +588,16 @@
         <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="K3" s="1">
         <v>812</v>
@@ -608,7 +605,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -626,16 +623,16 @@
         <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K4" s="1">
         <v>326</v>
@@ -643,7 +640,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
@@ -655,19 +652,19 @@
         <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>15</v>
@@ -678,13 +675,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -696,13 +693,13 @@
         <v>15</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>15</v>
@@ -713,13 +710,13 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -731,10 +728,10 @@
         <v>15</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>12</v>
@@ -748,13 +745,13 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>12</v>
@@ -763,16 +760,16 @@
         <v>14</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>15</v>
@@ -783,10 +780,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>21</v>
@@ -795,19 +792,19 @@
         <v>13</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>15</v>
@@ -818,13 +815,13 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>12</v>
@@ -836,10 +833,10 @@
         <v>15</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>12</v>
@@ -853,13 +850,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -868,16 +865,16 @@
         <v>14</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>15</v>

</xml_diff>